<commit_message>
small changes to glucose and insulin
</commit_message>
<xml_diff>
--- a/data/glucose/fingerstick.xlsx
+++ b/data/glucose/fingerstick.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kristili\R\ribose-paper\data\glucose\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krist\OneDrive\Documents\ribose-paper\data\glucose\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E60716B-8E8F-4018-BD7C-3D62434023D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06BC9B8A-FA7B-4B33-B678-7F22F3EECDA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1830" yWindow="1830" windowWidth="21600" windowHeight="11040" xr2:uid="{4965D424-3668-A246-8E22-DC40EB08FD9E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4965D424-3668-A246-8E22-DC40EB08FD9E}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="17">
   <si>
     <t>subject</t>
   </si>
@@ -120,11 +120,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,8 +440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77056ED4-E251-D342-B487-7CFC87EF20C8}">
   <dimension ref="A1:I196"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32:G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -451,7 +450,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -524,11 +523,11 @@
       <c r="E3" t="s">
         <v>8</v>
       </c>
-      <c r="F3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" t="s">
-        <v>8</v>
+      <c r="F3">
+        <v>3.56</v>
+      </c>
+      <c r="G3">
+        <v>2.38</v>
       </c>
       <c r="H3" t="s">
         <v>9</v>
@@ -727,11 +726,11 @@
       <c r="E10" t="s">
         <v>8</v>
       </c>
-      <c r="F10" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" t="s">
-        <v>8</v>
+      <c r="F10">
+        <v>3.56</v>
+      </c>
+      <c r="G10">
+        <v>2.38</v>
       </c>
       <c r="H10" t="s">
         <v>13</v>
@@ -959,11 +958,11 @@
       <c r="E18" t="s">
         <v>8</v>
       </c>
-      <c r="F18" t="s">
-        <v>8</v>
-      </c>
-      <c r="G18" t="s">
-        <v>8</v>
+      <c r="F18">
+        <v>4.21</v>
+      </c>
+      <c r="G18">
+        <v>1.24</v>
       </c>
       <c r="H18" t="s">
         <v>13</v>
@@ -1162,11 +1161,11 @@
       <c r="E25" t="s">
         <v>8</v>
       </c>
-      <c r="F25" t="s">
-        <v>8</v>
-      </c>
-      <c r="G25" t="s">
-        <v>8</v>
+      <c r="F25">
+        <v>4.21</v>
+      </c>
+      <c r="G25">
+        <v>1.24</v>
       </c>
       <c r="H25" t="s">
         <v>9</v>
@@ -1394,11 +1393,11 @@
       <c r="E33" t="s">
         <v>8</v>
       </c>
-      <c r="F33" t="s">
-        <v>8</v>
-      </c>
-      <c r="G33" t="s">
-        <v>8</v>
+      <c r="F33">
+        <v>3.6</v>
+      </c>
+      <c r="G33">
+        <v>2.23</v>
       </c>
       <c r="H33" t="s">
         <v>13</v>
@@ -1597,11 +1596,11 @@
       <c r="E40" t="s">
         <v>8</v>
       </c>
-      <c r="F40" t="s">
-        <v>8</v>
-      </c>
-      <c r="G40" t="s">
-        <v>8</v>
+      <c r="F40">
+        <v>3.6</v>
+      </c>
+      <c r="G40">
+        <v>2.23</v>
       </c>
       <c r="H40" t="s">
         <v>9</v>

</xml_diff>